<commit_message>
cambios y agregado de S3
</commit_message>
<xml_diff>
--- a/archivos_ejemplo/excel_prueba/pocos.xlsx
+++ b/archivos_ejemplo/excel_prueba/pocos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferro\OneDrive\Escritorio\Mejor_ninez\archivos_ejemplo\excel_prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B580A1-EE7C-49AB-B900-E662B1FCA65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7057BDE5-927B-4DD1-91FA-91ED71DCB9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>codNNA</t>
   </si>
@@ -244,7 +244,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -265,11 +265,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -278,11 +289,48 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -312,41 +360,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -361,7 +374,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3043A38-A63D-476F-9BF1-1FFCEEA2AC6D}" name="Tabla1" displayName="Tabla1" ref="A1:W3" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3043A38-A63D-476F-9BF1-1FFCEEA2AC6D}" name="Tabla1" displayName="Tabla1" ref="A1:W3" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
   <autoFilter ref="A1:W3" xr:uid="{A3043A38-A63D-476F-9BF1-1FFCEEA2AC6D}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{0465EC0A-A3C3-4E31-AA67-3B04499768AB}" name="codNNA"/>
@@ -655,23 +668,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8:V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.109375" customWidth="1"/>
     <col min="12" max="12" width="9.77734375" customWidth="1"/>
     <col min="14" max="14" width="13.88671875" customWidth="1"/>
@@ -683,7 +696,7 @@
     <col min="20" max="20" width="17.88671875" customWidth="1"/>
     <col min="21" max="21" width="9.77734375" customWidth="1"/>
     <col min="22" max="22" width="12.21875" customWidth="1"/>
-    <col min="23" max="23" width="16.5546875" customWidth="1"/>
+    <col min="23" max="23" width="40.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -899,9 +912,80 @@
         <v>56</v>
       </c>
     </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4965665</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1591408</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="5">
+        <v>45259</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4">
+        <v>16</v>
+      </c>
+      <c r="S4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A3">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  <conditionalFormatting sqref="A1:A4">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>